<commit_message>
Oprava useku na lichem zhlavi.
</commit_message>
<xml_diff>
--- a/Cejc_MTB_v1.xlsx
+++ b/Cejc_MTB_v1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="194">
   <si>
     <t>MTB 1</t>
   </si>
@@ -155,9 +155,6 @@
     <t>U6SA</t>
   </si>
   <si>
-    <t>v 1.0</t>
-  </si>
-  <si>
     <t>Seznam MTB Čejč</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>V13-</t>
   </si>
   <si>
-    <t>Sc2a</t>
-  </si>
-  <si>
     <t>Osvětlení 1</t>
   </si>
   <si>
@@ -597,6 +591,18 @@
   </si>
   <si>
     <t>Trať lichý směr</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>v 1.1</t>
+  </si>
+  <si>
+    <t>První úsek lichého záhlaví</t>
+  </si>
+  <si>
+    <t>ZahlL1</t>
   </si>
 </sst>
 </file>
@@ -1812,6 +1818,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1821,6 +1830,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1830,180 +1842,183 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2070,6 +2085,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2135,18 +2153,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2465,16 +2471,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
+      <c r="A1" s="131" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -2482,14 +2488,14 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -2498,7 +2504,7 @@
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
-        <v>44</v>
+        <v>191</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2524,38 +2530,38 @@
       <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="84"/>
     </row>
     <row r="6" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="87"/>
     </row>
     <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26"/>
       <c r="B7" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="86">
+      <c r="C7" s="89">
         <v>25</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="37"/>
       <c r="H7" s="29"/>
     </row>
@@ -2564,12 +2570,12 @@
       <c r="B8" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
+      <c r="C8" s="90" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
       <c r="G8" s="31"/>
       <c r="H8" s="29"/>
     </row>
@@ -2578,12 +2584,12 @@
       <c r="B9" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
       <c r="G9" s="31"/>
       <c r="H9" s="29"/>
     </row>
@@ -2592,12 +2598,12 @@
       <c r="B10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="89" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
+      <c r="C10" s="92" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
       <c r="G10" s="10"/>
       <c r="H10" s="29"/>
     </row>
@@ -2612,106 +2618,116 @@
       <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="130"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132" t="s">
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="136"/>
     </row>
     <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
         <v>0</v>
       </c>
-      <c r="B13" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="E13" s="33">
         <v>0</v>
       </c>
-      <c r="F13" s="134" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="135"/>
-      <c r="H13" s="136"/>
+      <c r="F13" s="137" t="s">
+        <v>190</v>
+      </c>
+      <c r="G13" s="138"/>
+      <c r="H13" s="139"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>1</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="62"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="E14" s="34">
         <v>1</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="76"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>2</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="62"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="E15" s="34">
         <v>2</v>
       </c>
-      <c r="F15" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="127"/>
+      <c r="F15" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="100"/>
+      <c r="H15" s="129"/>
     </row>
     <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>3</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="62"/>
-      <c r="D16" s="60"/>
+      <c r="D16" s="60" t="s">
+        <v>51</v>
+      </c>
       <c r="E16" s="34">
         <v>3</v>
       </c>
       <c r="F16" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="97"/>
-      <c r="H16" s="127"/>
+        <v>79</v>
+      </c>
+      <c r="G16" s="100"/>
+      <c r="H16" s="129"/>
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>4</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="28"/>
+        <v>63</v>
+      </c>
+      <c r="C17" s="130"/>
+      <c r="D17" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="E17" s="34">
         <v>4</v>
       </c>
       <c r="F17" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="97"/>
-      <c r="H17" s="127"/>
+        <v>78</v>
+      </c>
+      <c r="G17" s="100"/>
+      <c r="H17" s="129"/>
       <c r="I17" s="21"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
@@ -2721,16 +2737,18 @@
         <v>5</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="28"/>
+        <v>64</v>
+      </c>
+      <c r="C18" s="130"/>
+      <c r="D18" s="28" t="s">
+        <v>53</v>
+      </c>
       <c r="E18" s="34">
         <v>5</v>
       </c>
       <c r="F18" s="61"/>
       <c r="G18" s="62"/>
-      <c r="H18" s="72"/>
+      <c r="H18" s="64"/>
       <c r="I18" s="21"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -2741,16 +2759,18 @@
         <v>6</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="28"/>
+        <v>65</v>
+      </c>
+      <c r="C19" s="130"/>
+      <c r="D19" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="E19" s="34">
         <v>6</v>
       </c>
-      <c r="F19" s="71"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="62"/>
-      <c r="H19" s="72"/>
+      <c r="H19" s="64"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2758,162 +2778,164 @@
         <v>7</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="28"/>
+        <v>66</v>
+      </c>
+      <c r="C20" s="130"/>
+      <c r="D20" s="28" t="s">
+        <v>55</v>
+      </c>
       <c r="E20" s="34">
         <v>7</v>
       </c>
       <c r="F20" s="61"/>
       <c r="G20" s="62"/>
-      <c r="H20" s="72"/>
+      <c r="H20" s="64"/>
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>8</v>
       </c>
-      <c r="B21" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="113"/>
+      <c r="B21" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="78"/>
+      <c r="D21" s="115"/>
       <c r="E21" s="34">
         <v>8</v>
       </c>
-      <c r="F21" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="75"/>
-      <c r="H21" s="113"/>
+      <c r="F21" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="78"/>
+      <c r="H21" s="115"/>
       <c r="M21" s="6"/>
     </row>
     <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>9</v>
       </c>
-      <c r="B22" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="113"/>
+      <c r="B22" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="78"/>
+      <c r="D22" s="115"/>
       <c r="E22" s="34">
         <v>9</v>
       </c>
-      <c r="F22" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" s="75"/>
-      <c r="H22" s="113"/>
+      <c r="F22" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="78"/>
+      <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>10</v>
       </c>
-      <c r="B23" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="113"/>
+      <c r="B23" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="78"/>
+      <c r="D23" s="115"/>
       <c r="E23" s="34">
         <v>10</v>
       </c>
-      <c r="F23" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="75"/>
-      <c r="H23" s="113"/>
+      <c r="F23" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="78"/>
+      <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>11</v>
       </c>
-      <c r="B24" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="75"/>
-      <c r="D24" s="113"/>
+      <c r="B24" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="78"/>
+      <c r="D24" s="115"/>
       <c r="E24" s="34">
         <v>11</v>
       </c>
-      <c r="F24" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="75"/>
-      <c r="H24" s="113"/>
+      <c r="F24" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="78"/>
+      <c r="H24" s="115"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>12</v>
       </c>
-      <c r="B25" s="100" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="101"/>
-      <c r="D25" s="102"/>
+      <c r="B25" s="102" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="103"/>
+      <c r="D25" s="104"/>
       <c r="E25" s="34">
         <v>12</v>
       </c>
-      <c r="F25" s="100" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="101"/>
-      <c r="H25" s="102"/>
+      <c r="F25" s="102" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="103"/>
+      <c r="H25" s="104"/>
     </row>
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>13</v>
       </c>
-      <c r="B26" s="103" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="104"/>
+      <c r="B26" s="105" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="105"/>
+      <c r="D26" s="106"/>
       <c r="E26" s="34">
         <v>13</v>
       </c>
-      <c r="F26" s="103" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="103"/>
-      <c r="H26" s="104"/>
+      <c r="F26" s="105" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="105"/>
+      <c r="H26" s="106"/>
     </row>
     <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>14</v>
       </c>
-      <c r="B27" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="104"/>
+      <c r="B27" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
       <c r="E27" s="34">
         <v>14</v>
       </c>
-      <c r="F27" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="103"/>
-      <c r="H27" s="104"/>
+      <c r="F27" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="105"/>
+      <c r="H27" s="106"/>
     </row>
     <row r="28" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>15</v>
       </c>
-      <c r="B28" s="105" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="105"/>
-      <c r="D28" s="106"/>
+      <c r="B28" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="107"/>
+      <c r="D28" s="108"/>
       <c r="E28" s="35">
         <v>15</v>
       </c>
-      <c r="F28" s="105" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="105"/>
-      <c r="H28" s="106"/>
+      <c r="F28" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="107"/>
+      <c r="H28" s="108"/>
     </row>
     <row r="29" spans="1:13" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2927,38 +2949,38 @@
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:13" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="81"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="84"/>
     </row>
     <row r="31" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="82"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="84"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="B32" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="85">
+      <c r="C32" s="88">
         <v>26</v>
       </c>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
       <c r="G32" s="37"/>
       <c r="H32" s="29"/>
     </row>
@@ -2967,12 +2989,12 @@
       <c r="B33" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="117" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
+      <c r="C33" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
       <c r="G33" s="31"/>
       <c r="H33" s="29"/>
     </row>
@@ -2981,12 +3003,12 @@
       <c r="B34" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
       <c r="G34" s="31"/>
       <c r="H34" s="29"/>
     </row>
@@ -2995,12 +3017,12 @@
       <c r="B35" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
+      <c r="C35" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="10"/>
       <c r="H35" s="29"/>
     </row>
@@ -3015,82 +3037,90 @@
       <c r="H36" s="29"/>
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="92"/>
-      <c r="E37" s="93" t="s">
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="91"/>
-      <c r="G37" s="91"/>
-      <c r="H37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="97"/>
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17">
         <v>0</v>
       </c>
-      <c r="B38" s="95" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="96"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="98" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="99"/>
+      <c r="D38" s="27" t="s">
+        <v>80</v>
+      </c>
       <c r="E38" s="40">
         <v>0</v>
       </c>
       <c r="F38" s="61"/>
       <c r="G38" s="62"/>
-      <c r="H38" s="72"/>
+      <c r="H38" s="64"/>
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>1</v>
       </c>
       <c r="B39" s="61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C39" s="62"/>
-      <c r="D39" s="28"/>
+      <c r="D39" s="28" t="s">
+        <v>81</v>
+      </c>
       <c r="E39" s="41">
         <v>1</v>
       </c>
       <c r="F39" s="61"/>
       <c r="G39" s="62"/>
-      <c r="H39" s="72"/>
+      <c r="H39" s="64"/>
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>2</v>
       </c>
       <c r="B40" s="61" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="62"/>
-      <c r="D40" s="28"/>
+      <c r="D40" s="28" t="s">
+        <v>82</v>
+      </c>
       <c r="E40" s="41">
         <v>2</v>
       </c>
       <c r="F40" s="61"/>
       <c r="G40" s="62"/>
-      <c r="H40" s="72"/>
+      <c r="H40" s="64"/>
     </row>
     <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>3</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41" s="62"/>
-      <c r="D41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>83</v>
+      </c>
       <c r="E41" s="41">
         <v>3</v>
       </c>
       <c r="F41" s="61"/>
       <c r="G41" s="62"/>
-      <c r="H41" s="72"/>
+      <c r="H41" s="64"/>
     </row>
     <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
@@ -3104,7 +3134,7 @@
       </c>
       <c r="F42" s="61"/>
       <c r="G42" s="62"/>
-      <c r="H42" s="72"/>
+      <c r="H42" s="64"/>
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
@@ -3118,60 +3148,60 @@
       </c>
       <c r="F43" s="61"/>
       <c r="G43" s="62"/>
-      <c r="H43" s="72"/>
+      <c r="H43" s="64"/>
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>6</v>
       </c>
       <c r="B44" s="61"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="98"/>
+      <c r="C44" s="100"/>
+      <c r="D44" s="101"/>
       <c r="E44" s="41">
         <v>6</v>
       </c>
-      <c r="F44" s="71"/>
+      <c r="F44" s="73"/>
       <c r="G44" s="62"/>
-      <c r="H44" s="72"/>
+      <c r="H44" s="64"/>
     </row>
     <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>7</v>
       </c>
       <c r="B45" s="61"/>
-      <c r="C45" s="97"/>
-      <c r="D45" s="98"/>
+      <c r="C45" s="100"/>
+      <c r="D45" s="101"/>
       <c r="E45" s="41">
         <v>7</v>
       </c>
-      <c r="F45" s="71"/>
+      <c r="F45" s="73"/>
       <c r="G45" s="62"/>
-      <c r="H45" s="72"/>
+      <c r="H45" s="64"/>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>8</v>
       </c>
-      <c r="B46" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="66"/>
+      <c r="B46" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="66"/>
+      <c r="D46" s="67"/>
       <c r="E46" s="34">
         <v>8</v>
       </c>
-      <c r="F46" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="G46" s="65"/>
-      <c r="H46" s="66"/>
+      <c r="F46" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="66"/>
+      <c r="H46" s="67"/>
     </row>
     <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>9</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C47" s="62"/>
       <c r="D47" s="63"/>
@@ -3179,7 +3209,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G47" s="62"/>
       <c r="H47" s="63"/>
@@ -3196,7 +3226,7 @@
       </c>
       <c r="F48" s="61"/>
       <c r="G48" s="62"/>
-      <c r="H48" s="72"/>
+      <c r="H48" s="64"/>
     </row>
     <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
@@ -3210,63 +3240,63 @@
       </c>
       <c r="F49" s="61"/>
       <c r="G49" s="62"/>
-      <c r="H49" s="72"/>
+      <c r="H49" s="64"/>
     </row>
     <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>12</v>
       </c>
-      <c r="B50" s="118"/>
-      <c r="C50" s="119"/>
-      <c r="D50" s="120"/>
+      <c r="B50" s="120"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="122"/>
       <c r="E50" s="34">
         <v>12</v>
       </c>
       <c r="F50" s="61"/>
       <c r="G50" s="62"/>
-      <c r="H50" s="72"/>
+      <c r="H50" s="64"/>
     </row>
     <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>13</v>
       </c>
-      <c r="B51" s="118"/>
-      <c r="C51" s="119"/>
-      <c r="D51" s="120"/>
+      <c r="B51" s="120"/>
+      <c r="C51" s="121"/>
+      <c r="D51" s="122"/>
       <c r="E51" s="34">
         <v>13</v>
       </c>
       <c r="F51" s="61"/>
       <c r="G51" s="62"/>
-      <c r="H51" s="72"/>
+      <c r="H51" s="64"/>
     </row>
     <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>14</v>
       </c>
-      <c r="B52" s="124"/>
-      <c r="C52" s="125"/>
-      <c r="D52" s="126"/>
+      <c r="B52" s="126"/>
+      <c r="C52" s="127"/>
+      <c r="D52" s="128"/>
       <c r="E52" s="34">
         <v>14</v>
       </c>
-      <c r="F52" s="114"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="115"/>
+      <c r="F52" s="116"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="68"/>
     </row>
     <row r="53" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>15</v>
       </c>
-      <c r="B53" s="121"/>
-      <c r="C53" s="122"/>
-      <c r="D53" s="123"/>
+      <c r="B53" s="123"/>
+      <c r="C53" s="124"/>
+      <c r="D53" s="125"/>
       <c r="E53" s="35">
         <v>15</v>
       </c>
-      <c r="F53" s="116"/>
-      <c r="G53" s="110"/>
-      <c r="H53" s="111"/>
+      <c r="F53" s="118"/>
+      <c r="G53" s="112"/>
+      <c r="H53" s="113"/>
     </row>
     <row r="54" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
@@ -3279,38 +3309,38 @@
       <c r="H54" s="45"/>
     </row>
     <row r="55" spans="1:8" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="79" t="s">
+      <c r="A55" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="80"/>
-      <c r="C55" s="80"/>
-      <c r="D55" s="80"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="80"/>
-      <c r="G55" s="80"/>
-      <c r="H55" s="81"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="84"/>
     </row>
     <row r="56" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="82"/>
-      <c r="B56" s="83"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="83"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="83"/>
-      <c r="H56" s="84"/>
+      <c r="A56" s="85"/>
+      <c r="B56" s="86"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="86"/>
+      <c r="H56" s="87"/>
     </row>
     <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="36"/>
       <c r="B57" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="85">
+      <c r="C57" s="88">
         <v>27</v>
       </c>
-      <c r="D57" s="86"/>
-      <c r="E57" s="86"/>
-      <c r="F57" s="86"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="89"/>
       <c r="G57" s="48"/>
       <c r="H57" s="29"/>
     </row>
@@ -3319,12 +3349,12 @@
       <c r="B58" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="70" t="s">
-        <v>59</v>
-      </c>
-      <c r="D58" s="87"/>
-      <c r="E58" s="87"/>
-      <c r="F58" s="87"/>
+      <c r="C58" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="90"/>
+      <c r="E58" s="90"/>
+      <c r="F58" s="90"/>
       <c r="G58" s="47"/>
       <c r="H58" s="29"/>
     </row>
@@ -3333,12 +3363,12 @@
       <c r="B59" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="70" t="s">
+      <c r="C59" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D59" s="87"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="87"/>
+      <c r="D59" s="90"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="90"/>
       <c r="G59" s="47"/>
       <c r="H59" s="29"/>
     </row>
@@ -3347,12 +3377,12 @@
       <c r="B60" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="D60" s="89"/>
-      <c r="E60" s="89"/>
-      <c r="F60" s="89"/>
+      <c r="C60" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="92"/>
+      <c r="E60" s="92"/>
+      <c r="F60" s="92"/>
       <c r="G60" s="10"/>
       <c r="H60" s="29"/>
     </row>
@@ -3367,146 +3397,158 @@
       <c r="H61" s="29"/>
     </row>
     <row r="62" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="90" t="s">
+      <c r="A62" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="91"/>
-      <c r="C62" s="91"/>
-      <c r="D62" s="92"/>
-      <c r="E62" s="93" t="s">
+      <c r="B62" s="94"/>
+      <c r="C62" s="94"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="91"/>
-      <c r="G62" s="91"/>
-      <c r="H62" s="94"/>
+      <c r="F62" s="94"/>
+      <c r="G62" s="94"/>
+      <c r="H62" s="97"/>
     </row>
     <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="17">
         <v>0</v>
       </c>
       <c r="B63" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="99"/>
-      <c r="D63" s="28"/>
+        <v>92</v>
+      </c>
+      <c r="C63" s="117"/>
+      <c r="D63" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="E63" s="40">
         <v>0</v>
       </c>
-      <c r="F63" s="74"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="76"/>
+      <c r="F63" s="77"/>
+      <c r="G63" s="78"/>
+      <c r="H63" s="79"/>
     </row>
     <row r="64" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>1</v>
       </c>
       <c r="B64" s="61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C64" s="62"/>
-      <c r="D64" s="28"/>
+      <c r="D64" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="E64" s="41">
         <v>1</v>
       </c>
-      <c r="F64" s="74"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="76"/>
+      <c r="F64" s="77"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="79"/>
     </row>
     <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <v>2</v>
       </c>
       <c r="B65" s="61" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C65" s="62"/>
-      <c r="D65" s="56"/>
+      <c r="D65" s="56" t="s">
+        <v>88</v>
+      </c>
       <c r="E65" s="41">
         <v>2</v>
       </c>
-      <c r="F65" s="74"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="76"/>
+      <c r="F65" s="77"/>
+      <c r="G65" s="78"/>
+      <c r="H65" s="79"/>
     </row>
     <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>3</v>
       </c>
       <c r="B66" s="61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C66" s="62"/>
-      <c r="D66" s="28"/>
+      <c r="D66" s="28" t="s">
+        <v>89</v>
+      </c>
       <c r="E66" s="41">
         <v>3</v>
       </c>
-      <c r="F66" s="74"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="76"/>
+      <c r="F66" s="77"/>
+      <c r="G66" s="78"/>
+      <c r="H66" s="79"/>
     </row>
     <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>4</v>
       </c>
       <c r="B67" s="61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C67" s="62"/>
-      <c r="D67" s="56"/>
+      <c r="D67" s="56" t="s">
+        <v>90</v>
+      </c>
       <c r="E67" s="41">
         <v>4</v>
       </c>
-      <c r="F67" s="71"/>
+      <c r="F67" s="73"/>
       <c r="G67" s="62"/>
-      <c r="H67" s="72"/>
+      <c r="H67" s="64"/>
     </row>
     <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>5</v>
       </c>
       <c r="B68" s="61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C68" s="62"/>
-      <c r="D68" s="56"/>
+      <c r="D68" s="56" t="s">
+        <v>91</v>
+      </c>
       <c r="E68" s="41">
         <v>5</v>
       </c>
-      <c r="F68" s="71"/>
+      <c r="F68" s="73"/>
       <c r="G68" s="62"/>
-      <c r="H68" s="72"/>
+      <c r="H68" s="64"/>
     </row>
     <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>6</v>
       </c>
       <c r="B69" s="61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C69" s="62"/>
       <c r="D69" s="28"/>
       <c r="E69" s="41">
         <v>6</v>
       </c>
-      <c r="F69" s="71"/>
+      <c r="F69" s="73"/>
       <c r="G69" s="62"/>
-      <c r="H69" s="72"/>
+      <c r="H69" s="64"/>
     </row>
     <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>7</v>
       </c>
       <c r="B70" s="61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C70" s="62"/>
       <c r="D70" s="56"/>
       <c r="E70" s="41">
         <v>7</v>
       </c>
-      <c r="F70" s="71"/>
+      <c r="F70" s="73"/>
       <c r="G70" s="62"/>
-      <c r="H70" s="72"/>
+      <c r="H70" s="64"/>
     </row>
     <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
@@ -3520,7 +3562,7 @@
       </c>
       <c r="F71" s="61"/>
       <c r="G71" s="62"/>
-      <c r="H71" s="72"/>
+      <c r="H71" s="64"/>
     </row>
     <row r="72" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
@@ -3534,7 +3576,7 @@
       </c>
       <c r="F72" s="61"/>
       <c r="G72" s="62"/>
-      <c r="H72" s="72"/>
+      <c r="H72" s="64"/>
     </row>
     <row r="73" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
@@ -3548,7 +3590,7 @@
       </c>
       <c r="F73" s="61"/>
       <c r="G73" s="62"/>
-      <c r="H73" s="72"/>
+      <c r="H73" s="64"/>
     </row>
     <row r="74" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
@@ -3562,7 +3604,7 @@
       </c>
       <c r="F74" s="61"/>
       <c r="G74" s="62"/>
-      <c r="H74" s="72"/>
+      <c r="H74" s="64"/>
     </row>
     <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
@@ -3576,7 +3618,7 @@
       </c>
       <c r="F75" s="61"/>
       <c r="G75" s="62"/>
-      <c r="H75" s="72"/>
+      <c r="H75" s="64"/>
     </row>
     <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
@@ -3590,35 +3632,35 @@
       </c>
       <c r="F76" s="61"/>
       <c r="G76" s="62"/>
-      <c r="H76" s="72"/>
+      <c r="H76" s="64"/>
     </row>
     <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <v>14</v>
       </c>
-      <c r="B77" s="114"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="66"/>
+      <c r="B77" s="116"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="67"/>
       <c r="E77" s="34">
         <v>14</v>
       </c>
-      <c r="F77" s="114"/>
-      <c r="G77" s="65"/>
-      <c r="H77" s="115"/>
+      <c r="F77" s="116"/>
+      <c r="G77" s="66"/>
+      <c r="H77" s="68"/>
     </row>
     <row r="78" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19">
         <v>15</v>
       </c>
-      <c r="B78" s="112"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="69"/>
+      <c r="B78" s="114"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="71"/>
       <c r="E78" s="35">
         <v>15</v>
       </c>
-      <c r="F78" s="110"/>
-      <c r="G78" s="110"/>
-      <c r="H78" s="111"/>
+      <c r="F78" s="112"/>
+      <c r="G78" s="112"/>
+      <c r="H78" s="113"/>
     </row>
     <row r="79" spans="1:8" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="38"/>
@@ -3631,38 +3673,38 @@
       <c r="H79" s="25"/>
     </row>
     <row r="80" spans="1:8" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="79" t="s">
+      <c r="A80" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="80"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
-      <c r="E80" s="80"/>
-      <c r="F80" s="80"/>
-      <c r="G80" s="80"/>
-      <c r="H80" s="81"/>
+      <c r="B80" s="83"/>
+      <c r="C80" s="83"/>
+      <c r="D80" s="83"/>
+      <c r="E80" s="83"/>
+      <c r="F80" s="83"/>
+      <c r="G80" s="83"/>
+      <c r="H80" s="84"/>
     </row>
     <row r="81" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="82"/>
-      <c r="B81" s="83"/>
-      <c r="C81" s="83"/>
-      <c r="D81" s="83"/>
-      <c r="E81" s="83"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="83"/>
-      <c r="H81" s="84"/>
+      <c r="A81" s="85"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="86"/>
+      <c r="E81" s="86"/>
+      <c r="F81" s="86"/>
+      <c r="G81" s="86"/>
+      <c r="H81" s="87"/>
     </row>
     <row r="82" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="36"/>
       <c r="B82" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C82" s="85">
+      <c r="C82" s="88">
         <v>28</v>
       </c>
-      <c r="D82" s="86"/>
-      <c r="E82" s="86"/>
-      <c r="F82" s="86"/>
+      <c r="D82" s="89"/>
+      <c r="E82" s="89"/>
+      <c r="F82" s="89"/>
       <c r="G82" s="48"/>
       <c r="H82" s="29"/>
     </row>
@@ -3671,12 +3713,12 @@
       <c r="B83" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C83" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D83" s="87"/>
-      <c r="E83" s="87"/>
-      <c r="F83" s="87"/>
+      <c r="C83" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D83" s="90"/>
+      <c r="E83" s="90"/>
+      <c r="F83" s="90"/>
       <c r="G83" s="47"/>
       <c r="H83" s="29"/>
     </row>
@@ -3685,12 +3727,12 @@
       <c r="B84" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="70" t="s">
+      <c r="C84" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D84" s="87"/>
-      <c r="E84" s="87"/>
-      <c r="F84" s="87"/>
+      <c r="D84" s="90"/>
+      <c r="E84" s="90"/>
+      <c r="F84" s="90"/>
       <c r="G84" s="47"/>
       <c r="H84" s="29"/>
     </row>
@@ -3699,12 +3741,12 @@
       <c r="B85" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="88" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="89"/>
-      <c r="E85" s="89"/>
-      <c r="F85" s="89"/>
+      <c r="C85" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="92"/>
+      <c r="E85" s="92"/>
+      <c r="F85" s="92"/>
       <c r="G85" s="10"/>
       <c r="H85" s="29"/>
     </row>
@@ -3719,156 +3761,172 @@
       <c r="H86" s="29"/>
     </row>
     <row r="87" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="90" t="s">
+      <c r="A87" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="91"/>
-      <c r="C87" s="91"/>
-      <c r="D87" s="92"/>
-      <c r="E87" s="93" t="s">
+      <c r="B87" s="94"/>
+      <c r="C87" s="94"/>
+      <c r="D87" s="95"/>
+      <c r="E87" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F87" s="91"/>
-      <c r="G87" s="91"/>
-      <c r="H87" s="94"/>
+      <c r="F87" s="94"/>
+      <c r="G87" s="94"/>
+      <c r="H87" s="97"/>
     </row>
     <row r="88" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="17">
         <v>0</v>
       </c>
-      <c r="B88" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="C88" s="96"/>
-      <c r="D88" s="27"/>
+      <c r="B88" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C88" s="99"/>
+      <c r="D88" s="27" t="s">
+        <v>100</v>
+      </c>
       <c r="E88" s="40">
         <v>0</v>
       </c>
-      <c r="F88" s="74"/>
-      <c r="G88" s="75"/>
-      <c r="H88" s="76"/>
+      <c r="F88" s="77"/>
+      <c r="G88" s="78"/>
+      <c r="H88" s="79"/>
     </row>
     <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="18">
         <v>1</v>
       </c>
       <c r="B89" s="61" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C89" s="62"/>
-      <c r="D89" s="28"/>
+      <c r="D89" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="E89" s="41">
         <v>1</v>
       </c>
-      <c r="F89" s="74"/>
-      <c r="G89" s="75"/>
-      <c r="H89" s="76"/>
+      <c r="F89" s="77"/>
+      <c r="G89" s="78"/>
+      <c r="H89" s="79"/>
     </row>
     <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="18">
         <v>2</v>
       </c>
       <c r="B90" s="61" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C90" s="62"/>
-      <c r="D90" s="28"/>
+      <c r="D90" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="E90" s="41">
         <v>2</v>
       </c>
-      <c r="F90" s="74"/>
-      <c r="G90" s="75"/>
-      <c r="H90" s="76"/>
+      <c r="F90" s="77"/>
+      <c r="G90" s="78"/>
+      <c r="H90" s="79"/>
     </row>
     <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="18">
         <v>3</v>
       </c>
-      <c r="B91" s="77" t="s">
-        <v>109</v>
-      </c>
-      <c r="C91" s="78"/>
-      <c r="D91" s="28"/>
+      <c r="B91" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" s="81"/>
+      <c r="D91" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="E91" s="41">
         <v>3</v>
       </c>
-      <c r="F91" s="74"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="76"/>
+      <c r="F91" s="77"/>
+      <c r="G91" s="78"/>
+      <c r="H91" s="79"/>
     </row>
     <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="18">
         <v>4</v>
       </c>
       <c r="B92" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="C92" s="99"/>
-      <c r="D92" s="28"/>
+        <v>111</v>
+      </c>
+      <c r="C92" s="117"/>
+      <c r="D92" s="28" t="s">
+        <v>108</v>
+      </c>
       <c r="E92" s="41">
         <v>4</v>
       </c>
-      <c r="F92" s="71"/>
+      <c r="F92" s="73"/>
       <c r="G92" s="62"/>
-      <c r="H92" s="72"/>
+      <c r="H92" s="64"/>
     </row>
     <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="18">
         <v>5</v>
       </c>
       <c r="B93" s="61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C93" s="62"/>
-      <c r="D93" s="28"/>
+      <c r="D93" s="28" t="s">
+        <v>109</v>
+      </c>
       <c r="E93" s="41">
         <v>5</v>
       </c>
-      <c r="F93" s="71"/>
+      <c r="F93" s="73"/>
       <c r="G93" s="62"/>
-      <c r="H93" s="72"/>
+      <c r="H93" s="64"/>
     </row>
     <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="18">
         <v>6</v>
       </c>
       <c r="B94" s="61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C94" s="62"/>
-      <c r="D94" s="28"/>
+      <c r="D94" s="28" t="s">
+        <v>110</v>
+      </c>
       <c r="E94" s="41">
         <v>6</v>
       </c>
-      <c r="F94" s="71"/>
+      <c r="F94" s="73"/>
       <c r="G94" s="62"/>
-      <c r="H94" s="72"/>
+      <c r="H94" s="64"/>
     </row>
     <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="18">
         <v>7</v>
       </c>
       <c r="B95" s="61" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C95" s="62"/>
-      <c r="D95" s="28"/>
+      <c r="D95" s="28" t="s">
+        <v>124</v>
+      </c>
       <c r="E95" s="41">
         <v>7</v>
       </c>
-      <c r="F95" s="71"/>
+      <c r="F95" s="73"/>
       <c r="G95" s="62"/>
-      <c r="H95" s="72"/>
+      <c r="H95" s="64"/>
     </row>
     <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="18">
         <v>8</v>
       </c>
-      <c r="B96" s="64" t="s">
+      <c r="B96" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C96" s="65"/>
-      <c r="D96" s="66"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="67"/>
       <c r="E96" s="34">
         <v>8</v>
       </c>
@@ -3876,7 +3934,7 @@
         <v>40</v>
       </c>
       <c r="G96" s="62"/>
-      <c r="H96" s="72"/>
+      <c r="H96" s="64"/>
     </row>
     <row r="97" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="18">
@@ -3894,14 +3952,14 @@
         <v>41</v>
       </c>
       <c r="G97" s="62"/>
-      <c r="H97" s="72"/>
+      <c r="H97" s="64"/>
     </row>
     <row r="98" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="18">
         <v>10</v>
       </c>
       <c r="B98" s="61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C98" s="62"/>
       <c r="D98" s="63"/>
@@ -3909,17 +3967,17 @@
         <v>10</v>
       </c>
       <c r="F98" s="61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G98" s="62"/>
-      <c r="H98" s="72"/>
+      <c r="H98" s="64"/>
     </row>
     <row r="99" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="18">
         <v>11</v>
       </c>
       <c r="B99" s="61" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C99" s="62"/>
       <c r="D99" s="63"/>
@@ -3927,10 +3985,10 @@
         <v>11</v>
       </c>
       <c r="F99" s="61" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G99" s="62"/>
-      <c r="H99" s="72"/>
+      <c r="H99" s="64"/>
     </row>
     <row r="100" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="18">
@@ -3944,14 +4002,14 @@
       </c>
       <c r="F100" s="61"/>
       <c r="G100" s="62"/>
-      <c r="H100" s="72"/>
+      <c r="H100" s="64"/>
     </row>
     <row r="101" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="18">
         <v>13</v>
       </c>
       <c r="B101" s="57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C101" s="58"/>
       <c r="D101" s="59"/>
@@ -3960,7 +4018,7 @@
       </c>
       <c r="F101" s="61"/>
       <c r="G101" s="62"/>
-      <c r="H101" s="72"/>
+      <c r="H101" s="64"/>
     </row>
     <row r="102" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="18">
@@ -3974,25 +4032,25 @@
       <c r="E102" s="34">
         <v>14</v>
       </c>
-      <c r="F102" s="114"/>
-      <c r="G102" s="65"/>
-      <c r="H102" s="115"/>
+      <c r="F102" s="116"/>
+      <c r="G102" s="66"/>
+      <c r="H102" s="68"/>
     </row>
     <row r="103" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="19">
         <v>15</v>
       </c>
-      <c r="B103" s="107" t="s">
+      <c r="B103" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="C103" s="108"/>
-      <c r="D103" s="109"/>
+      <c r="C103" s="110"/>
+      <c r="D103" s="111"/>
       <c r="E103" s="35">
         <v>15</v>
       </c>
-      <c r="F103" s="110"/>
-      <c r="G103" s="110"/>
-      <c r="H103" s="111"/>
+      <c r="F103" s="112"/>
+      <c r="G103" s="112"/>
+      <c r="H103" s="113"/>
     </row>
     <row r="104" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -4006,38 +4064,38 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="80"/>
-      <c r="C105" s="80"/>
-      <c r="D105" s="80"/>
-      <c r="E105" s="80"/>
-      <c r="F105" s="80"/>
-      <c r="G105" s="80"/>
-      <c r="H105" s="81"/>
+      <c r="A105" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" s="83"/>
+      <c r="C105" s="83"/>
+      <c r="D105" s="83"/>
+      <c r="E105" s="83"/>
+      <c r="F105" s="83"/>
+      <c r="G105" s="83"/>
+      <c r="H105" s="84"/>
     </row>
     <row r="106" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="82"/>
-      <c r="B106" s="83"/>
-      <c r="C106" s="83"/>
-      <c r="D106" s="83"/>
-      <c r="E106" s="83"/>
-      <c r="F106" s="83"/>
-      <c r="G106" s="83"/>
-      <c r="H106" s="84"/>
+      <c r="A106" s="85"/>
+      <c r="B106" s="86"/>
+      <c r="C106" s="86"/>
+      <c r="D106" s="86"/>
+      <c r="E106" s="86"/>
+      <c r="F106" s="86"/>
+      <c r="G106" s="86"/>
+      <c r="H106" s="87"/>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="36"/>
       <c r="B107" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C107" s="85">
+      <c r="C107" s="88">
         <v>29</v>
       </c>
-      <c r="D107" s="86"/>
-      <c r="E107" s="86"/>
-      <c r="F107" s="86"/>
+      <c r="D107" s="89"/>
+      <c r="E107" s="89"/>
+      <c r="F107" s="89"/>
       <c r="G107" s="48"/>
       <c r="H107" s="29"/>
     </row>
@@ -4046,12 +4104,12 @@
       <c r="B108" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C108" s="70" t="s">
-        <v>145</v>
-      </c>
-      <c r="D108" s="87"/>
-      <c r="E108" s="87"/>
-      <c r="F108" s="87"/>
+      <c r="C108" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="D108" s="90"/>
+      <c r="E108" s="90"/>
+      <c r="F108" s="90"/>
       <c r="G108" s="47"/>
       <c r="H108" s="29"/>
     </row>
@@ -4060,12 +4118,12 @@
       <c r="B109" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C109" s="70" t="s">
+      <c r="C109" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D109" s="87"/>
-      <c r="E109" s="87"/>
-      <c r="F109" s="87"/>
+      <c r="D109" s="90"/>
+      <c r="E109" s="90"/>
+      <c r="F109" s="90"/>
       <c r="G109" s="47"/>
       <c r="H109" s="29"/>
     </row>
@@ -4074,12 +4132,12 @@
       <c r="B110" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C110" s="88" t="s">
-        <v>50</v>
-      </c>
-      <c r="D110" s="89"/>
-      <c r="E110" s="89"/>
-      <c r="F110" s="89"/>
+      <c r="C110" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D110" s="92"/>
+      <c r="E110" s="92"/>
+      <c r="F110" s="92"/>
       <c r="G110" s="10"/>
       <c r="H110" s="29"/>
     </row>
@@ -4094,290 +4152,290 @@
       <c r="H111" s="29"/>
     </row>
     <row r="112" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="90" t="s">
+      <c r="A112" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B112" s="91"/>
-      <c r="C112" s="91"/>
-      <c r="D112" s="92"/>
-      <c r="E112" s="93" t="s">
+      <c r="B112" s="94"/>
+      <c r="C112" s="94"/>
+      <c r="D112" s="95"/>
+      <c r="E112" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F112" s="91"/>
-      <c r="G112" s="91"/>
-      <c r="H112" s="94"/>
+      <c r="F112" s="94"/>
+      <c r="G112" s="94"/>
+      <c r="H112" s="97"/>
     </row>
     <row r="113" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="17">
         <v>0</v>
       </c>
-      <c r="B113" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="C113" s="96"/>
+      <c r="B113" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="C113" s="99"/>
       <c r="D113" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E113" s="40">
         <v>0</v>
       </c>
-      <c r="F113" s="74"/>
-      <c r="G113" s="75"/>
-      <c r="H113" s="76"/>
+      <c r="F113" s="77"/>
+      <c r="G113" s="78"/>
+      <c r="H113" s="79"/>
     </row>
     <row r="114" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="18">
         <v>1</v>
       </c>
       <c r="B114" s="61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C114" s="62"/>
       <c r="D114" s="28" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="E114" s="41">
         <v>1</v>
       </c>
-      <c r="F114" s="74"/>
-      <c r="G114" s="75"/>
-      <c r="H114" s="76"/>
+      <c r="F114" s="77"/>
+      <c r="G114" s="78"/>
+      <c r="H114" s="79"/>
     </row>
     <row r="115" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="18">
         <v>2</v>
       </c>
       <c r="B115" s="61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C115" s="62"/>
       <c r="D115" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E115" s="41">
         <v>2</v>
       </c>
-      <c r="F115" s="74"/>
-      <c r="G115" s="75"/>
-      <c r="H115" s="76"/>
+      <c r="F115" s="77"/>
+      <c r="G115" s="78"/>
+      <c r="H115" s="79"/>
     </row>
     <row r="116" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="18">
         <v>3</v>
       </c>
-      <c r="B116" s="77" t="s">
-        <v>132</v>
-      </c>
-      <c r="C116" s="78"/>
+      <c r="B116" s="80" t="s">
+        <v>130</v>
+      </c>
+      <c r="C116" s="81"/>
       <c r="D116" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E116" s="41">
         <v>3</v>
       </c>
-      <c r="F116" s="74"/>
-      <c r="G116" s="75"/>
-      <c r="H116" s="76"/>
+      <c r="F116" s="77"/>
+      <c r="G116" s="78"/>
+      <c r="H116" s="79"/>
     </row>
     <row r="117" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="18">
         <v>4</v>
       </c>
-      <c r="B117" s="70"/>
-      <c r="C117" s="172"/>
-      <c r="D117" s="173"/>
+      <c r="B117" s="74"/>
+      <c r="C117" s="75"/>
+      <c r="D117" s="76"/>
       <c r="E117" s="41">
         <v>4</v>
       </c>
-      <c r="F117" s="71"/>
+      <c r="F117" s="73"/>
       <c r="G117" s="62"/>
-      <c r="H117" s="72"/>
+      <c r="H117" s="64"/>
     </row>
     <row r="118" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="18">
         <v>5</v>
       </c>
-      <c r="B118" s="70"/>
-      <c r="C118" s="172"/>
-      <c r="D118" s="173"/>
+      <c r="B118" s="74"/>
+      <c r="C118" s="75"/>
+      <c r="D118" s="76"/>
       <c r="E118" s="41">
         <v>5</v>
       </c>
-      <c r="F118" s="71"/>
+      <c r="F118" s="73"/>
       <c r="G118" s="62"/>
-      <c r="H118" s="72"/>
+      <c r="H118" s="64"/>
     </row>
     <row r="119" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="18">
         <v>6</v>
       </c>
-      <c r="B119" s="70"/>
-      <c r="C119" s="172"/>
-      <c r="D119" s="173"/>
+      <c r="B119" s="74"/>
+      <c r="C119" s="75"/>
+      <c r="D119" s="76"/>
       <c r="E119" s="41">
         <v>6</v>
       </c>
-      <c r="F119" s="71"/>
+      <c r="F119" s="73"/>
       <c r="G119" s="62"/>
-      <c r="H119" s="72"/>
+      <c r="H119" s="64"/>
     </row>
     <row r="120" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="18">
         <v>7</v>
       </c>
-      <c r="B120" s="70"/>
-      <c r="C120" s="172"/>
-      <c r="D120" s="173"/>
+      <c r="B120" s="74"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="76"/>
       <c r="E120" s="41">
         <v>7</v>
       </c>
-      <c r="F120" s="71"/>
+      <c r="F120" s="73"/>
       <c r="G120" s="62"/>
-      <c r="H120" s="72"/>
+      <c r="H120" s="64"/>
     </row>
     <row r="121" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="18">
         <v>8</v>
       </c>
       <c r="B121" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="C121" s="97"/>
-      <c r="D121" s="98"/>
+        <v>117</v>
+      </c>
+      <c r="C121" s="100"/>
+      <c r="D121" s="101"/>
       <c r="E121" s="34">
         <v>8</v>
       </c>
       <c r="F121" s="61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G121" s="62"/>
-      <c r="H121" s="72"/>
+      <c r="H121" s="64"/>
     </row>
     <row r="122" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="18">
         <v>9</v>
       </c>
       <c r="B122" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C122" s="97"/>
-      <c r="D122" s="98"/>
+        <v>118</v>
+      </c>
+      <c r="C122" s="100"/>
+      <c r="D122" s="101"/>
       <c r="E122" s="34">
         <v>9</v>
       </c>
       <c r="F122" s="61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G122" s="62"/>
-      <c r="H122" s="72"/>
+      <c r="H122" s="64"/>
     </row>
     <row r="123" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="18">
         <v>10</v>
       </c>
       <c r="B123" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="C123" s="97"/>
-      <c r="D123" s="98"/>
+        <v>119</v>
+      </c>
+      <c r="C123" s="100"/>
+      <c r="D123" s="101"/>
       <c r="E123" s="34">
         <v>10</v>
       </c>
       <c r="F123" s="61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G123" s="62"/>
-      <c r="H123" s="72"/>
+      <c r="H123" s="64"/>
     </row>
     <row r="124" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="18">
         <v>11</v>
       </c>
       <c r="B124" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="C124" s="97"/>
-      <c r="D124" s="98"/>
+        <v>120</v>
+      </c>
+      <c r="C124" s="100"/>
+      <c r="D124" s="101"/>
       <c r="E124" s="34">
         <v>11</v>
       </c>
       <c r="F124" s="61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G124" s="62"/>
-      <c r="H124" s="72"/>
+      <c r="H124" s="64"/>
     </row>
     <row r="125" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="18">
         <v>12</v>
       </c>
       <c r="B125" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="C125" s="97"/>
-      <c r="D125" s="98"/>
+        <v>131</v>
+      </c>
+      <c r="C125" s="100"/>
+      <c r="D125" s="101"/>
       <c r="E125" s="34">
         <v>12</v>
       </c>
       <c r="F125" s="61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G125" s="62"/>
-      <c r="H125" s="72"/>
+      <c r="H125" s="64"/>
     </row>
     <row r="126" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="18">
         <v>13</v>
       </c>
       <c r="B126" s="61" t="s">
-        <v>134</v>
-      </c>
-      <c r="C126" s="97"/>
-      <c r="D126" s="98"/>
+        <v>132</v>
+      </c>
+      <c r="C126" s="100"/>
+      <c r="D126" s="101"/>
       <c r="E126" s="34">
         <v>13</v>
       </c>
       <c r="F126" s="61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G126" s="62"/>
-      <c r="H126" s="72"/>
+      <c r="H126" s="64"/>
     </row>
     <row r="127" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="18">
         <v>14</v>
       </c>
-      <c r="B127" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C127" s="65"/>
-      <c r="D127" s="66"/>
+      <c r="B127" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C127" s="66"/>
+      <c r="D127" s="67"/>
       <c r="E127" s="34">
         <v>14</v>
       </c>
-      <c r="F127" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="G127" s="65"/>
-      <c r="H127" s="115"/>
+      <c r="F127" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="G127" s="66"/>
+      <c r="H127" s="68"/>
     </row>
     <row r="128" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="19">
         <v>15</v>
       </c>
-      <c r="B128" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="C128" s="68"/>
-      <c r="D128" s="69"/>
+      <c r="B128" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="C128" s="70"/>
+      <c r="D128" s="71"/>
       <c r="E128" s="35">
         <v>15</v>
       </c>
-      <c r="F128" s="67" t="s">
-        <v>124</v>
-      </c>
-      <c r="G128" s="68"/>
-      <c r="H128" s="174"/>
+      <c r="F128" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="G128" s="70"/>
+      <c r="H128" s="72"/>
     </row>
     <row r="129" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
@@ -4391,38 +4449,38 @@
       <c r="I129" s="4"/>
     </row>
     <row r="130" spans="1:9" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="79" t="s">
-        <v>136</v>
-      </c>
-      <c r="B130" s="80"/>
-      <c r="C130" s="80"/>
-      <c r="D130" s="80"/>
-      <c r="E130" s="80"/>
-      <c r="F130" s="80"/>
-      <c r="G130" s="80"/>
-      <c r="H130" s="81"/>
+      <c r="A130" s="82" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" s="83"/>
+      <c r="C130" s="83"/>
+      <c r="D130" s="83"/>
+      <c r="E130" s="83"/>
+      <c r="F130" s="83"/>
+      <c r="G130" s="83"/>
+      <c r="H130" s="84"/>
     </row>
     <row r="131" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="82"/>
-      <c r="B131" s="83"/>
-      <c r="C131" s="83"/>
-      <c r="D131" s="83"/>
-      <c r="E131" s="83"/>
-      <c r="F131" s="83"/>
-      <c r="G131" s="83"/>
-      <c r="H131" s="84"/>
+      <c r="A131" s="85"/>
+      <c r="B131" s="86"/>
+      <c r="C131" s="86"/>
+      <c r="D131" s="86"/>
+      <c r="E131" s="86"/>
+      <c r="F131" s="86"/>
+      <c r="G131" s="86"/>
+      <c r="H131" s="87"/>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="36"/>
       <c r="B132" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C132" s="85">
+      <c r="C132" s="88">
         <v>30</v>
       </c>
-      <c r="D132" s="86"/>
-      <c r="E132" s="86"/>
-      <c r="F132" s="86"/>
+      <c r="D132" s="89"/>
+      <c r="E132" s="89"/>
+      <c r="F132" s="89"/>
       <c r="G132" s="48"/>
       <c r="H132" s="29"/>
     </row>
@@ -4431,12 +4489,12 @@
       <c r="B133" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C133" s="70" t="s">
-        <v>146</v>
-      </c>
-      <c r="D133" s="87"/>
-      <c r="E133" s="87"/>
-      <c r="F133" s="87"/>
+      <c r="C133" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="D133" s="90"/>
+      <c r="E133" s="90"/>
+      <c r="F133" s="90"/>
       <c r="G133" s="47"/>
       <c r="H133" s="29"/>
     </row>
@@ -4445,12 +4503,12 @@
       <c r="B134" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C134" s="70" t="s">
+      <c r="C134" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="D134" s="87"/>
-      <c r="E134" s="87"/>
-      <c r="F134" s="87"/>
+      <c r="D134" s="90"/>
+      <c r="E134" s="90"/>
+      <c r="F134" s="90"/>
       <c r="G134" s="47"/>
       <c r="H134" s="29"/>
     </row>
@@ -4459,12 +4517,12 @@
       <c r="B135" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C135" s="88" t="s">
-        <v>135</v>
-      </c>
-      <c r="D135" s="89"/>
-      <c r="E135" s="89"/>
-      <c r="F135" s="89"/>
+      <c r="C135" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="D135" s="92"/>
+      <c r="E135" s="92"/>
+      <c r="F135" s="92"/>
       <c r="G135" s="10"/>
       <c r="H135" s="29"/>
     </row>
@@ -4479,45 +4537,45 @@
       <c r="H136" s="29"/>
     </row>
     <row r="137" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="90" t="s">
+      <c r="A137" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B137" s="91"/>
-      <c r="C137" s="91"/>
-      <c r="D137" s="92"/>
-      <c r="E137" s="93" t="s">
+      <c r="B137" s="94"/>
+      <c r="C137" s="94"/>
+      <c r="D137" s="95"/>
+      <c r="E137" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F137" s="91"/>
-      <c r="G137" s="91"/>
-      <c r="H137" s="94"/>
+      <c r="F137" s="94"/>
+      <c r="G137" s="94"/>
+      <c r="H137" s="97"/>
     </row>
     <row r="138" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="17">
         <v>0</v>
       </c>
-      <c r="B138" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="C138" s="96"/>
+      <c r="B138" s="98" t="s">
+        <v>135</v>
+      </c>
+      <c r="C138" s="99"/>
       <c r="D138" s="27" t="s">
         <v>29</v>
       </c>
       <c r="E138" s="40">
         <v>0</v>
       </c>
-      <c r="F138" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="G138" s="75"/>
-      <c r="H138" s="76"/>
+      <c r="F138" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="G138" s="78"/>
+      <c r="H138" s="79"/>
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="18">
         <v>1</v>
       </c>
       <c r="B139" s="61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C139" s="62"/>
       <c r="D139" s="28" t="s">
@@ -4526,16 +4584,16 @@
       <c r="E139" s="41">
         <v>1</v>
       </c>
-      <c r="F139" s="74"/>
-      <c r="G139" s="75"/>
-      <c r="H139" s="76"/>
+      <c r="F139" s="77"/>
+      <c r="G139" s="78"/>
+      <c r="H139" s="79"/>
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="18">
         <v>2</v>
       </c>
       <c r="B140" s="61" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C140" s="62"/>
       <c r="D140" s="28" t="s">
@@ -4544,93 +4602,93 @@
       <c r="E140" s="41">
         <v>2</v>
       </c>
-      <c r="F140" s="74"/>
-      <c r="G140" s="75"/>
-      <c r="H140" s="76"/>
+      <c r="F140" s="77"/>
+      <c r="G140" s="78"/>
+      <c r="H140" s="79"/>
     </row>
     <row r="141" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="18">
         <v>3</v>
       </c>
-      <c r="B141" s="77" t="s">
-        <v>140</v>
-      </c>
-      <c r="C141" s="78"/>
+      <c r="B141" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C141" s="81"/>
       <c r="D141" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E141" s="41">
         <v>3</v>
       </c>
-      <c r="F141" s="74"/>
-      <c r="G141" s="75"/>
-      <c r="H141" s="76"/>
+      <c r="F141" s="77"/>
+      <c r="G141" s="78"/>
+      <c r="H141" s="79"/>
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="18">
         <v>4</v>
       </c>
-      <c r="B142" s="70"/>
-      <c r="C142" s="172"/>
-      <c r="D142" s="173"/>
+      <c r="B142" s="74"/>
+      <c r="C142" s="75"/>
+      <c r="D142" s="76"/>
       <c r="E142" s="41">
         <v>4</v>
       </c>
-      <c r="F142" s="71"/>
+      <c r="F142" s="73"/>
       <c r="G142" s="62"/>
-      <c r="H142" s="72"/>
+      <c r="H142" s="64"/>
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="18">
         <v>5</v>
       </c>
-      <c r="B143" s="70"/>
-      <c r="C143" s="172"/>
-      <c r="D143" s="173"/>
+      <c r="B143" s="74"/>
+      <c r="C143" s="75"/>
+      <c r="D143" s="76"/>
       <c r="E143" s="41">
         <v>5</v>
       </c>
-      <c r="F143" s="71"/>
+      <c r="F143" s="73"/>
       <c r="G143" s="62"/>
-      <c r="H143" s="72"/>
+      <c r="H143" s="64"/>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="18">
         <v>6</v>
       </c>
-      <c r="B144" s="70"/>
-      <c r="C144" s="172"/>
-      <c r="D144" s="173"/>
+      <c r="B144" s="74"/>
+      <c r="C144" s="75"/>
+      <c r="D144" s="76"/>
       <c r="E144" s="41">
         <v>6</v>
       </c>
-      <c r="F144" s="71"/>
+      <c r="F144" s="73"/>
       <c r="G144" s="62"/>
-      <c r="H144" s="72"/>
+      <c r="H144" s="64"/>
     </row>
     <row r="145" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="18">
         <v>7</v>
       </c>
-      <c r="B145" s="70"/>
-      <c r="C145" s="172"/>
-      <c r="D145" s="173"/>
+      <c r="B145" s="74"/>
+      <c r="C145" s="75"/>
+      <c r="D145" s="76"/>
       <c r="E145" s="41">
         <v>7</v>
       </c>
-      <c r="F145" s="71"/>
+      <c r="F145" s="73"/>
       <c r="G145" s="62"/>
-      <c r="H145" s="72"/>
+      <c r="H145" s="64"/>
     </row>
     <row r="146" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="18">
         <v>8</v>
       </c>
-      <c r="B146" s="64" t="s">
+      <c r="B146" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C146" s="65"/>
-      <c r="D146" s="66"/>
+      <c r="C146" s="66"/>
+      <c r="D146" s="67"/>
       <c r="E146" s="34">
         <v>8</v>
       </c>
@@ -4638,7 +4696,7 @@
         <v>32</v>
       </c>
       <c r="G146" s="62"/>
-      <c r="H146" s="72"/>
+      <c r="H146" s="64"/>
     </row>
     <row r="147" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="18">
@@ -4656,7 +4714,7 @@
         <v>33</v>
       </c>
       <c r="G147" s="62"/>
-      <c r="H147" s="72"/>
+      <c r="H147" s="64"/>
     </row>
     <row r="148" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="18">
@@ -4674,7 +4732,7 @@
         <v>31</v>
       </c>
       <c r="G148" s="62"/>
-      <c r="H148" s="72"/>
+      <c r="H148" s="64"/>
     </row>
     <row r="149" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="18">
@@ -4690,7 +4748,7 @@
       </c>
       <c r="F149" s="61"/>
       <c r="G149" s="62"/>
-      <c r="H149" s="72"/>
+      <c r="H149" s="64"/>
     </row>
     <row r="150" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="18">
@@ -4706,7 +4764,7 @@
       </c>
       <c r="F150" s="61"/>
       <c r="G150" s="62"/>
-      <c r="H150" s="72"/>
+      <c r="H150" s="64"/>
     </row>
     <row r="151" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="18">
@@ -4722,35 +4780,35 @@
       </c>
       <c r="F151" s="61"/>
       <c r="G151" s="62"/>
-      <c r="H151" s="72"/>
+      <c r="H151" s="64"/>
     </row>
     <row r="152" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="18">
         <v>14</v>
       </c>
-      <c r="B152" s="64"/>
-      <c r="C152" s="65"/>
-      <c r="D152" s="66"/>
+      <c r="B152" s="65"/>
+      <c r="C152" s="66"/>
+      <c r="D152" s="67"/>
       <c r="E152" s="34">
         <v>14</v>
       </c>
-      <c r="F152" s="64"/>
-      <c r="G152" s="65"/>
-      <c r="H152" s="115"/>
+      <c r="F152" s="65"/>
+      <c r="G152" s="66"/>
+      <c r="H152" s="68"/>
     </row>
     <row r="153" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="19">
         <v>15</v>
       </c>
-      <c r="B153" s="67"/>
-      <c r="C153" s="68"/>
-      <c r="D153" s="69"/>
+      <c r="B153" s="69"/>
+      <c r="C153" s="70"/>
+      <c r="D153" s="71"/>
       <c r="E153" s="35">
         <v>15</v>
       </c>
-      <c r="F153" s="67"/>
-      <c r="G153" s="68"/>
-      <c r="H153" s="174"/>
+      <c r="F153" s="69"/>
+      <c r="G153" s="70"/>
+      <c r="H153" s="72"/>
     </row>
     <row r="154" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5002,7 +5060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
@@ -5013,13 +5071,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
+      <c r="A1" s="131" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
       <c r="F1" s="42"/>
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
@@ -5030,11 +5088,11 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
       <c r="H2" s="42"/>
@@ -5045,13 +5103,13 @@
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
       <c r="H3" s="42"/>
@@ -5073,13 +5131,13 @@
       <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:13" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="158" t="s">
+      <c r="A5" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="159"/>
-      <c r="C5" s="159"/>
-      <c r="D5" s="159"/>
-      <c r="E5" s="159"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -5089,11 +5147,11 @@
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="175" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="150"/>
-      <c r="D6" s="151"/>
+      <c r="B6" s="153" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="154"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="12"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -5104,11 +5162,11 @@
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="149" t="s">
+      <c r="B7" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="149"/>
-      <c r="D7" s="117"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="119"/>
       <c r="E7" s="14"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -5119,11 +5177,11 @@
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="154" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="154"/>
-      <c r="D8" s="155"/>
+      <c r="B8" s="158" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="158"/>
+      <c r="D8" s="159"/>
       <c r="E8" s="16"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -5131,13 +5189,13 @@
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="130"/>
-      <c r="C9" s="130"/>
-      <c r="D9" s="130"/>
-      <c r="E9" s="152"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="26"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -5147,11 +5205,11 @@
       <c r="A10" s="17">
         <v>1</v>
       </c>
-      <c r="B10" s="95" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
+      <c r="B10" s="98" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
       <c r="E10" s="51" t="s">
         <v>25</v>
       </c>
@@ -5165,7 +5223,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
@@ -5182,12 +5240,12 @@
         <v>3</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
       <c r="E12" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="25"/>
@@ -5198,13 +5256,13 @@
       <c r="A13" s="19">
         <v>4</v>
       </c>
-      <c r="B13" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="25"/>
@@ -5223,13 +5281,13 @@
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:13" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="142" t="s">
+      <c r="A15" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="143"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="144"/>
+      <c r="B15" s="146"/>
+      <c r="C15" s="146"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="147"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
@@ -5239,11 +5297,11 @@
       <c r="A16" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="145" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
+      <c r="B16" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
       <c r="E16" s="12"/>
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
@@ -5254,11 +5312,11 @@
       <c r="A17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
       <c r="E17" s="14"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
@@ -5269,11 +5327,11 @@
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="155" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
+      <c r="B18" s="159" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="16"/>
       <c r="F18" s="24"/>
       <c r="G18" s="24"/>
@@ -5281,13 +5339,13 @@
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="94"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="24"/>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -5299,13 +5357,13 @@
       <c r="A20" s="17">
         <v>1</v>
       </c>
-      <c r="B20" s="95" t="s">
-        <v>161</v>
-      </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
+      <c r="B20" s="98" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99"/>
       <c r="E20" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
@@ -5319,12 +5377,12 @@
         <v>2</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C21" s="62"/>
       <c r="D21" s="62"/>
       <c r="E21" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="25"/>
@@ -5338,12 +5396,12 @@
         <v>3</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C22" s="62"/>
       <c r="D22" s="62"/>
       <c r="E22" s="54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
@@ -5356,13 +5414,13 @@
       <c r="A23" s="19">
         <v>4</v>
       </c>
-      <c r="B23" s="67" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="25"/>
@@ -5385,13 +5443,13 @@
       <c r="K24" s="43"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="142" t="s">
+      <c r="A25" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="147"/>
-      <c r="C25" s="147"/>
-      <c r="D25" s="147"/>
-      <c r="E25" s="148"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="151"/>
       <c r="F25" s="24"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -5403,11 +5461,11 @@
       <c r="A26" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="175" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="150"/>
-      <c r="D26" s="151"/>
+      <c r="B26" s="153" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="154"/>
+      <c r="D26" s="155"/>
       <c r="E26" s="12"/>
       <c r="F26" s="24"/>
       <c r="G26" s="25"/>
@@ -5420,11 +5478,11 @@
       <c r="A27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="149" t="s">
+      <c r="B27" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="149"/>
-      <c r="D27" s="117"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="119"/>
       <c r="E27" s="49"/>
       <c r="F27" s="24"/>
       <c r="G27" s="25"/>
@@ -5437,11 +5495,11 @@
       <c r="A28" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="153" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="154"/>
-      <c r="D28" s="155"/>
+      <c r="B28" s="157" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="158"/>
+      <c r="D28" s="159"/>
       <c r="E28" s="16"/>
       <c r="F28" s="24"/>
       <c r="G28" s="25"/>
@@ -5451,13 +5509,13 @@
       <c r="K28" s="43"/>
     </row>
     <row r="29" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="129" t="s">
+      <c r="A29" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="130"/>
-      <c r="C29" s="130"/>
-      <c r="D29" s="130"/>
-      <c r="E29" s="152"/>
+      <c r="B29" s="133"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="156"/>
       <c r="F29" s="24"/>
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
@@ -5469,13 +5527,13 @@
       <c r="A30" s="17">
         <v>1</v>
       </c>
-      <c r="B30" s="95" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
+      <c r="B30" s="98" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
       <c r="E30" s="53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="25"/>
@@ -5489,12 +5547,12 @@
         <v>2</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C31" s="62"/>
       <c r="D31" s="62"/>
       <c r="E31" s="54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="25"/>
@@ -5507,13 +5565,13 @@
       <c r="A32" s="18">
         <v>3</v>
       </c>
-      <c r="B32" s="77" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
+      <c r="B32" s="80" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="25"/>
@@ -5526,13 +5584,13 @@
       <c r="A33" s="19">
         <v>4</v>
       </c>
-      <c r="B33" s="67" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
+      <c r="B33" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
       <c r="E33" s="55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="24"/>
@@ -5551,13 +5609,13 @@
       <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="142" t="s">
+      <c r="A35" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="147"/>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="148"/>
+      <c r="B35" s="150"/>
+      <c r="C35" s="150"/>
+      <c r="D35" s="150"/>
+      <c r="E35" s="151"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
@@ -5567,11 +5625,11 @@
       <c r="A36" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="175" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" s="150"/>
-      <c r="D36" s="151"/>
+      <c r="B36" s="153" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="154"/>
+      <c r="D36" s="155"/>
       <c r="E36" s="12"/>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
@@ -5582,11 +5640,11 @@
       <c r="A37" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="149" t="s">
+      <c r="B37" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="149"/>
-      <c r="D37" s="117"/>
+      <c r="C37" s="152"/>
+      <c r="D37" s="119"/>
       <c r="E37" s="14"/>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
@@ -5597,11 +5655,11 @@
       <c r="A38" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="153" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="154"/>
-      <c r="D38" s="155"/>
+      <c r="B38" s="157" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="158"/>
+      <c r="D38" s="159"/>
       <c r="E38" s="16"/>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
@@ -5609,13 +5667,13 @@
       <c r="I38" s="24"/>
     </row>
     <row r="39" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="129" t="s">
+      <c r="A39" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="130"/>
-      <c r="C39" s="130"/>
-      <c r="D39" s="130"/>
-      <c r="E39" s="152"/>
+      <c r="B39" s="133"/>
+      <c r="C39" s="133"/>
+      <c r="D39" s="133"/>
+      <c r="E39" s="156"/>
       <c r="F39" s="24"/>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>
@@ -5625,11 +5683,11 @@
       <c r="A40" s="17">
         <v>1</v>
       </c>
-      <c r="B40" s="95" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" s="140"/>
-      <c r="D40" s="141"/>
+      <c r="B40" s="98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="143"/>
+      <c r="D40" s="144"/>
       <c r="E40" s="53" t="s">
         <v>23</v>
       </c>
@@ -5643,7 +5701,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="61" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C41" s="62"/>
       <c r="D41" s="62"/>
@@ -5660,12 +5718,12 @@
         <v>3</v>
       </c>
       <c r="B42" s="61" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C42" s="62"/>
       <c r="D42" s="62"/>
       <c r="E42" s="54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F42" s="24"/>
       <c r="G42" s="24"/>
@@ -5676,13 +5734,13 @@
       <c r="A43" s="19">
         <v>4</v>
       </c>
-      <c r="B43" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
+      <c r="B43" s="69" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F43" s="24"/>
       <c r="G43" s="24"/>
@@ -5691,13 +5749,13 @@
     </row>
     <row r="44" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="142" t="s">
+      <c r="A45" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="143"/>
-      <c r="C45" s="143"/>
-      <c r="D45" s="143"/>
-      <c r="E45" s="144"/>
+      <c r="B45" s="146"/>
+      <c r="C45" s="146"/>
+      <c r="D45" s="146"/>
+      <c r="E45" s="147"/>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
@@ -5707,11 +5765,11 @@
       <c r="A46" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="145" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="146"/>
-      <c r="D46" s="146"/>
+      <c r="B46" s="148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="149"/>
+      <c r="D46" s="149"/>
       <c r="E46" s="12"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
@@ -5722,11 +5780,11 @@
       <c r="A47" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="117" t="s">
+      <c r="B47" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
       <c r="E47" s="49"/>
       <c r="F47" s="24"/>
       <c r="G47" s="24"/>
@@ -5737,11 +5795,11 @@
       <c r="A48" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B48" s="139" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
+      <c r="B48" s="142" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
       <c r="E48" s="16"/>
       <c r="F48" s="24"/>
       <c r="G48" s="24"/>
@@ -5749,13 +5807,13 @@
       <c r="I48" s="24"/>
     </row>
     <row r="49" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="90" t="s">
+      <c r="A49" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="91"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="94"/>
+      <c r="B49" s="94"/>
+      <c r="C49" s="94"/>
+      <c r="D49" s="94"/>
+      <c r="E49" s="97"/>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
@@ -5765,13 +5823,13 @@
       <c r="A50" s="17">
         <v>1</v>
       </c>
-      <c r="B50" s="95" t="s">
-        <v>175</v>
-      </c>
-      <c r="C50" s="140"/>
-      <c r="D50" s="141"/>
+      <c r="B50" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="143"/>
+      <c r="D50" s="144"/>
       <c r="E50" s="53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
@@ -5783,12 +5841,12 @@
         <v>2</v>
       </c>
       <c r="B51" s="61" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" s="97"/>
-      <c r="D51" s="73"/>
+        <v>174</v>
+      </c>
+      <c r="C51" s="100"/>
+      <c r="D51" s="130"/>
       <c r="E51" s="54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
@@ -5800,8 +5858,8 @@
         <v>3</v>
       </c>
       <c r="B52" s="61"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="73"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="130"/>
       <c r="E52" s="54"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
@@ -5812,9 +5870,9 @@
       <c r="A53" s="19">
         <v>4</v>
       </c>
-      <c r="B53" s="67"/>
-      <c r="C53" s="137"/>
-      <c r="D53" s="138"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="140"/>
+      <c r="D53" s="141"/>
       <c r="E53" s="55"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
@@ -5823,13 +5881,13 @@
     </row>
     <row r="54" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="142" t="s">
+      <c r="A55" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="B55" s="143"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="143"/>
-      <c r="E55" s="144"/>
+      <c r="B55" s="146"/>
+      <c r="C55" s="146"/>
+      <c r="D55" s="146"/>
+      <c r="E55" s="147"/>
       <c r="F55" s="24"/>
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
@@ -5839,11 +5897,11 @@
       <c r="A56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="145" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" s="146"/>
-      <c r="D56" s="146"/>
+      <c r="B56" s="148" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="149"/>
+      <c r="D56" s="149"/>
       <c r="E56" s="12"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24"/>
@@ -5854,11 +5912,11 @@
       <c r="A57" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="117" t="s">
+      <c r="B57" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="87"/>
-      <c r="D57" s="87"/>
+      <c r="C57" s="90"/>
+      <c r="D57" s="90"/>
       <c r="E57" s="49"/>
       <c r="F57" s="24"/>
       <c r="G57" s="24"/>
@@ -5869,11 +5927,11 @@
       <c r="A58" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="139" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
+      <c r="B58" s="142" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="91"/>
+      <c r="D58" s="91"/>
       <c r="E58" s="16"/>
       <c r="F58" s="24"/>
       <c r="G58" s="24"/>
@@ -5881,13 +5939,13 @@
       <c r="I58" s="24"/>
     </row>
     <row r="59" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="90" t="s">
+      <c r="A59" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="91"/>
-      <c r="C59" s="91"/>
-      <c r="D59" s="91"/>
-      <c r="E59" s="94"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="97"/>
       <c r="F59" s="24"/>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
@@ -5897,13 +5955,13 @@
       <c r="A60" s="17">
         <v>1</v>
       </c>
-      <c r="B60" s="95" t="s">
-        <v>177</v>
-      </c>
-      <c r="C60" s="140"/>
-      <c r="D60" s="141"/>
+      <c r="B60" s="98" t="s">
+        <v>175</v>
+      </c>
+      <c r="C60" s="143"/>
+      <c r="D60" s="144"/>
       <c r="E60" s="53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F60" s="24"/>
       <c r="G60" s="24"/>
@@ -5915,12 +5973,12 @@
         <v>2</v>
       </c>
       <c r="B61" s="61" t="s">
-        <v>178</v>
-      </c>
-      <c r="C61" s="97"/>
-      <c r="D61" s="73"/>
+        <v>176</v>
+      </c>
+      <c r="C61" s="100"/>
+      <c r="D61" s="130"/>
       <c r="E61" s="54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F61" s="24"/>
       <c r="G61" s="24"/>
@@ -5932,12 +5990,12 @@
         <v>3</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>179</v>
-      </c>
-      <c r="C62" s="97"/>
-      <c r="D62" s="73"/>
+        <v>177</v>
+      </c>
+      <c r="C62" s="100"/>
+      <c r="D62" s="130"/>
       <c r="E62" s="54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F62" s="24"/>
       <c r="G62" s="24"/>
@@ -5948,13 +6006,13 @@
       <c r="A63" s="19">
         <v>4</v>
       </c>
-      <c r="B63" s="67" t="s">
-        <v>180</v>
-      </c>
-      <c r="C63" s="137"/>
-      <c r="D63" s="138"/>
+      <c r="B63" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" s="140"/>
+      <c r="D63" s="141"/>
       <c r="E63" s="55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F63" s="24"/>
       <c r="G63" s="24"/>
@@ -5963,13 +6021,13 @@
     </row>
     <row r="64" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="142" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="143"/>
-      <c r="C65" s="143"/>
-      <c r="D65" s="143"/>
-      <c r="E65" s="144"/>
+      <c r="A65" s="145" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="146"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="146"/>
+      <c r="E65" s="147"/>
       <c r="F65" s="24"/>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
@@ -5979,11 +6037,11 @@
       <c r="A66" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B66" s="145" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="146"/>
-      <c r="D66" s="146"/>
+      <c r="B66" s="148" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="149"/>
+      <c r="D66" s="149"/>
       <c r="E66" s="12"/>
       <c r="F66" s="24"/>
       <c r="G66" s="24"/>
@@ -5994,11 +6052,11 @@
       <c r="A67" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="117" t="s">
+      <c r="B67" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="87"/>
-      <c r="D67" s="87"/>
+      <c r="C67" s="90"/>
+      <c r="D67" s="90"/>
       <c r="E67" s="49"/>
       <c r="F67" s="24"/>
       <c r="G67" s="24"/>
@@ -6009,11 +6067,11 @@
       <c r="A68" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="139" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68" s="88"/>
-      <c r="D68" s="88"/>
+      <c r="B68" s="142" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" s="91"/>
+      <c r="D68" s="91"/>
       <c r="E68" s="16"/>
       <c r="F68" s="24"/>
       <c r="G68" s="24"/>
@@ -6021,13 +6079,13 @@
       <c r="I68" s="24"/>
     </row>
     <row r="69" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="90" t="s">
+      <c r="A69" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B69" s="91"/>
-      <c r="C69" s="91"/>
-      <c r="D69" s="91"/>
-      <c r="E69" s="94"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="94"/>
+      <c r="D69" s="94"/>
+      <c r="E69" s="97"/>
       <c r="F69" s="24"/>
       <c r="G69" s="24"/>
       <c r="H69" s="24"/>
@@ -6037,13 +6095,13 @@
       <c r="A70" s="17">
         <v>1</v>
       </c>
-      <c r="B70" s="95" t="s">
-        <v>181</v>
-      </c>
-      <c r="C70" s="140"/>
-      <c r="D70" s="141"/>
+      <c r="B70" s="98" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" s="143"/>
+      <c r="D70" s="144"/>
       <c r="E70" s="53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F70" s="24"/>
       <c r="G70" s="24"/>
@@ -6055,12 +6113,12 @@
         <v>2</v>
       </c>
       <c r="B71" s="61" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71" s="97"/>
-      <c r="D71" s="73"/>
+        <v>180</v>
+      </c>
+      <c r="C71" s="100"/>
+      <c r="D71" s="130"/>
       <c r="E71" s="54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F71" s="24"/>
       <c r="G71" s="24"/>
@@ -6072,12 +6130,12 @@
         <v>3</v>
       </c>
       <c r="B72" s="61" t="s">
-        <v>183</v>
-      </c>
-      <c r="C72" s="97"/>
-      <c r="D72" s="73"/>
+        <v>181</v>
+      </c>
+      <c r="C72" s="100"/>
+      <c r="D72" s="130"/>
       <c r="E72" s="54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F72" s="24"/>
       <c r="G72" s="24"/>
@@ -6088,13 +6146,13 @@
       <c r="A73" s="19">
         <v>4</v>
       </c>
-      <c r="B73" s="67" t="s">
-        <v>184</v>
-      </c>
-      <c r="C73" s="137"/>
-      <c r="D73" s="138"/>
+      <c r="B73" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="140"/>
+      <c r="D73" s="141"/>
       <c r="E73" s="55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F73" s="24"/>
       <c r="G73" s="24"/>
@@ -6103,13 +6161,13 @@
     </row>
     <row r="74" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="142" t="s">
-        <v>100</v>
-      </c>
-      <c r="B75" s="143"/>
-      <c r="C75" s="143"/>
-      <c r="D75" s="143"/>
-      <c r="E75" s="144"/>
+      <c r="A75" s="145" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="146"/>
+      <c r="C75" s="146"/>
+      <c r="D75" s="146"/>
+      <c r="E75" s="147"/>
       <c r="F75" s="24"/>
       <c r="G75" s="24"/>
       <c r="H75" s="24"/>
@@ -6119,11 +6177,11 @@
       <c r="A76" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="145" t="s">
-        <v>157</v>
-      </c>
-      <c r="C76" s="146"/>
-      <c r="D76" s="146"/>
+      <c r="B76" s="148" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="149"/>
+      <c r="D76" s="149"/>
       <c r="E76" s="12"/>
       <c r="F76" s="24"/>
       <c r="G76" s="24"/>
@@ -6134,11 +6192,11 @@
       <c r="A77" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="117" t="s">
+      <c r="B77" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="87"/>
-      <c r="D77" s="87"/>
+      <c r="C77" s="90"/>
+      <c r="D77" s="90"/>
       <c r="E77" s="49"/>
       <c r="F77" s="24"/>
       <c r="G77" s="24"/>
@@ -6149,11 +6207,11 @@
       <c r="A78" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="139" t="s">
-        <v>50</v>
-      </c>
-      <c r="C78" s="88"/>
-      <c r="D78" s="88"/>
+      <c r="B78" s="142" t="s">
+        <v>49</v>
+      </c>
+      <c r="C78" s="91"/>
+      <c r="D78" s="91"/>
       <c r="E78" s="16"/>
       <c r="F78" s="24"/>
       <c r="G78" s="24"/>
@@ -6161,13 +6219,13 @@
       <c r="I78" s="24"/>
     </row>
     <row r="79" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="90" t="s">
+      <c r="A79" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="91"/>
-      <c r="C79" s="91"/>
-      <c r="D79" s="91"/>
-      <c r="E79" s="94"/>
+      <c r="B79" s="94"/>
+      <c r="C79" s="94"/>
+      <c r="D79" s="94"/>
+      <c r="E79" s="97"/>
       <c r="F79" s="24"/>
       <c r="G79" s="24"/>
       <c r="H79" s="24"/>
@@ -6177,13 +6235,13 @@
       <c r="A80" s="17">
         <v>1</v>
       </c>
-      <c r="B80" s="95" t="s">
-        <v>185</v>
-      </c>
-      <c r="C80" s="140"/>
-      <c r="D80" s="141"/>
+      <c r="B80" s="98" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="143"/>
+      <c r="D80" s="144"/>
       <c r="E80" s="53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F80" s="24"/>
       <c r="G80" s="24"/>
@@ -6195,12 +6253,12 @@
         <v>2</v>
       </c>
       <c r="B81" s="61" t="s">
-        <v>184</v>
-      </c>
-      <c r="C81" s="97"/>
-      <c r="D81" s="73"/>
+        <v>192</v>
+      </c>
+      <c r="C81" s="100"/>
+      <c r="D81" s="130"/>
       <c r="E81" s="54" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="F81" s="24"/>
       <c r="G81" s="24"/>
@@ -6212,12 +6270,12 @@
         <v>3</v>
       </c>
       <c r="B82" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="C82" s="97"/>
-      <c r="D82" s="73"/>
+        <v>184</v>
+      </c>
+      <c r="C82" s="100"/>
+      <c r="D82" s="130"/>
       <c r="E82" s="54" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F82" s="24"/>
       <c r="G82" s="24"/>
@@ -6228,13 +6286,13 @@
       <c r="A83" s="19">
         <v>4</v>
       </c>
-      <c r="B83" s="67" t="s">
-        <v>187</v>
-      </c>
-      <c r="C83" s="137"/>
-      <c r="D83" s="138"/>
+      <c r="B83" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="C83" s="140"/>
+      <c r="D83" s="141"/>
       <c r="E83" s="55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24"/>
@@ -6243,13 +6301,13 @@
     </row>
     <row r="84" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:9" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="142" t="s">
-        <v>101</v>
-      </c>
-      <c r="B85" s="143"/>
-      <c r="C85" s="143"/>
-      <c r="D85" s="143"/>
-      <c r="E85" s="144"/>
+      <c r="A85" s="145" t="s">
+        <v>99</v>
+      </c>
+      <c r="B85" s="146"/>
+      <c r="C85" s="146"/>
+      <c r="D85" s="146"/>
+      <c r="E85" s="147"/>
       <c r="F85" s="24"/>
       <c r="G85" s="24"/>
       <c r="H85" s="24"/>
@@ -6259,11 +6317,11 @@
       <c r="A86" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="145" t="s">
-        <v>158</v>
-      </c>
-      <c r="C86" s="146"/>
-      <c r="D86" s="146"/>
+      <c r="B86" s="148" t="s">
+        <v>156</v>
+      </c>
+      <c r="C86" s="149"/>
+      <c r="D86" s="149"/>
       <c r="E86" s="12"/>
       <c r="F86" s="24"/>
       <c r="G86" s="24"/>
@@ -6274,11 +6332,11 @@
       <c r="A87" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="117" t="s">
+      <c r="B87" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="87"/>
-      <c r="D87" s="87"/>
+      <c r="C87" s="90"/>
+      <c r="D87" s="90"/>
       <c r="E87" s="49"/>
       <c r="F87" s="24"/>
       <c r="G87" s="24"/>
@@ -6289,11 +6347,11 @@
       <c r="A88" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B88" s="139" t="s">
-        <v>135</v>
-      </c>
-      <c r="C88" s="88"/>
-      <c r="D88" s="88"/>
+      <c r="B88" s="142" t="s">
+        <v>133</v>
+      </c>
+      <c r="C88" s="91"/>
+      <c r="D88" s="91"/>
       <c r="E88" s="16"/>
       <c r="F88" s="24"/>
       <c r="G88" s="24"/>
@@ -6301,13 +6359,13 @@
       <c r="I88" s="24"/>
     </row>
     <row r="89" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="90" t="s">
+      <c r="A89" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B89" s="91"/>
-      <c r="C89" s="91"/>
-      <c r="D89" s="91"/>
-      <c r="E89" s="94"/>
+      <c r="B89" s="94"/>
+      <c r="C89" s="94"/>
+      <c r="D89" s="94"/>
+      <c r="E89" s="97"/>
       <c r="F89" s="24"/>
       <c r="G89" s="24"/>
       <c r="H89" s="24"/>
@@ -6317,11 +6375,11 @@
       <c r="A90" s="17">
         <v>1</v>
       </c>
-      <c r="B90" s="95" t="s">
-        <v>188</v>
-      </c>
-      <c r="C90" s="140"/>
-      <c r="D90" s="141"/>
+      <c r="B90" s="98" t="s">
+        <v>186</v>
+      </c>
+      <c r="C90" s="143"/>
+      <c r="D90" s="144"/>
       <c r="E90" s="53" t="s">
         <v>29</v>
       </c>
@@ -6335,10 +6393,10 @@
         <v>2</v>
       </c>
       <c r="B91" s="61" t="s">
-        <v>189</v>
-      </c>
-      <c r="C91" s="97"/>
-      <c r="D91" s="73"/>
+        <v>187</v>
+      </c>
+      <c r="C91" s="100"/>
+      <c r="D91" s="130"/>
       <c r="E91" s="54" t="s">
         <v>28</v>
       </c>
@@ -6352,10 +6410,10 @@
         <v>3</v>
       </c>
       <c r="B92" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="C92" s="97"/>
-      <c r="D92" s="73"/>
+        <v>188</v>
+      </c>
+      <c r="C92" s="100"/>
+      <c r="D92" s="130"/>
       <c r="E92" s="54" t="s">
         <v>30</v>
       </c>
@@ -6368,11 +6426,11 @@
       <c r="A93" s="19">
         <v>4</v>
       </c>
-      <c r="B93" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="C93" s="137"/>
-      <c r="D93" s="138"/>
+      <c r="B93" s="69" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="140"/>
+      <c r="D93" s="141"/>
       <c r="E93" s="55" t="s">
         <v>21</v>
       </c>
@@ -6384,6 +6442,15 @@
     <row r="94" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="A89:E89"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:D61"/>
     <mergeCell ref="B62:D62"/>
@@ -6458,15 +6525,6 @@
     <mergeCell ref="B81:D81"/>
     <mergeCell ref="B82:D82"/>
     <mergeCell ref="B83:D83"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:D93"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6487,91 +6545,91 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
     </row>
     <row r="2" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128"/>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="170"/>
-      <c r="C3" s="170" t="s">
+      <c r="B3" s="174"/>
+      <c r="C3" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
-      <c r="I3" s="171"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="175"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="167" t="s">
+      <c r="A4" s="171" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="168"/>
-      <c r="C4" s="165" t="s">
+      <c r="B4" s="172"/>
+      <c r="C4" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="165"/>
-      <c r="I4" s="166"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="169"/>
+      <c r="I4" s="170"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="164"/>
-      <c r="B5" s="165"/>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
-      <c r="E5" s="165"/>
-      <c r="F5" s="165"/>
-      <c r="G5" s="165"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="166"/>
+      <c r="A5" s="168"/>
+      <c r="B5" s="169"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
+      <c r="H5" s="169"/>
+      <c r="I5" s="170"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="167"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="165"/>
-      <c r="F6" s="165"/>
-      <c r="G6" s="165"/>
-      <c r="H6" s="165"/>
-      <c r="I6" s="166"/>
+      <c r="A6" s="171"/>
+      <c r="B6" s="172"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="169"/>
+      <c r="H6" s="169"/>
+      <c r="I6" s="170"/>
     </row>
     <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="160"/>
-      <c r="B7" s="161"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="163"/>
+      <c r="A7" s="164"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
+      <c r="G7" s="166"/>
+      <c r="H7" s="166"/>
+      <c r="I7" s="167"/>
     </row>
     <row r="8" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>